<commit_message>
Added function to update ETF details
Function to update the ETF details such as AUM,Fundhouse name
</commit_message>
<xml_diff>
--- a/ETF_Data/ETFdetail_Dec_Combined.xlsx
+++ b/ETF_Data/ETFdetail_Dec_Combined.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Project/ETFAnalyser/ETF/ETF_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20996493-99FE-D245-B8B2-62260AEBBBBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664915E0-6839-D34B-9E0F-170C79C9D32D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$K$103</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="588">
   <si>
     <t>NAV</t>
   </si>
@@ -1712,13 +1715,85 @@
   </si>
   <si>
     <t>https://www.tickertape.in/etfs/motilal-oswal-nifty-midcap-100-etf-M100</t>
+  </si>
+  <si>
+    <t>ETF Fund house</t>
+  </si>
+  <si>
+    <t>Invesco</t>
+  </si>
+  <si>
+    <t>UTI </t>
+  </si>
+  <si>
+    <t>LIC Mutual Fund</t>
+  </si>
+  <si>
+    <t>Mirae Asset Financial Group</t>
+  </si>
+  <si>
+    <t>DSP</t>
+  </si>
+  <si>
+    <t>IDFC</t>
+  </si>
+  <si>
+    <t>IDBI</t>
+  </si>
+  <si>
+    <t>Edelweiss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reliance Nippon Life </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edelweiss   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tata   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axis     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICICI Prudential     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDFC   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motilal Oswal     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantum    Pvt  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBI Mutual Fund     </t>
+  </si>
+  <si>
+    <t>Kotak Mahindra      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aditya Birla Sun Life AMC  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indiabulls Housing Finance  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aditya Birla Sun Life </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aditya Birla Sun Life  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mirae Asset Financial </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1730,6 +1805,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1764,16 +1847,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2074,18 +2160,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView tabSelected="1" topLeftCell="C55" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="69.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.83203125" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="69.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2111,13 +2206,16 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2143,13 +2241,16 @@
         <v>17</v>
       </c>
       <c r="I2" t="s">
+        <v>572</v>
+      </c>
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2175,13 +2276,16 @@
         <v>24</v>
       </c>
       <c r="I3" t="s">
+        <v>576</v>
+      </c>
+      <c r="J3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -2207,13 +2311,16 @@
         <v>32</v>
       </c>
       <c r="I4" t="s">
+        <v>577</v>
+      </c>
+      <c r="J4" t="s">
         <v>33</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2239,13 +2346,16 @@
         <v>38</v>
       </c>
       <c r="I5" t="s">
+        <v>565</v>
+      </c>
+      <c r="J5" t="s">
         <v>39</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2271,13 +2381,16 @@
         <v>46</v>
       </c>
       <c r="I6" t="s">
+        <v>578</v>
+      </c>
+      <c r="J6" t="s">
         <v>47</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2303,13 +2416,16 @@
         <v>52</v>
       </c>
       <c r="I7" t="s">
+        <v>574</v>
+      </c>
+      <c r="J7" t="s">
         <v>53</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2335,13 +2451,16 @@
         <v>59</v>
       </c>
       <c r="I8" t="s">
+        <v>578</v>
+      </c>
+      <c r="J8" t="s">
         <v>60</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2367,13 +2486,16 @@
         <v>64</v>
       </c>
       <c r="I9" t="s">
+        <v>575</v>
+      </c>
+      <c r="J9" t="s">
         <v>65</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2399,13 +2521,16 @@
         <v>69</v>
       </c>
       <c r="I10" t="s">
+        <v>566</v>
+      </c>
+      <c r="J10" t="s">
         <v>70</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -2431,13 +2556,16 @@
         <v>76</v>
       </c>
       <c r="I11" t="s">
+        <v>566</v>
+      </c>
+      <c r="J11" t="s">
         <v>77</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2463,13 +2591,16 @@
         <v>84</v>
       </c>
       <c r="I12" t="s">
+        <v>567</v>
+      </c>
+      <c r="J12" t="s">
         <v>85</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2495,13 +2626,16 @@
         <v>89</v>
       </c>
       <c r="I13" t="s">
+        <v>581</v>
+      </c>
+      <c r="J13" t="s">
         <v>90</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>92</v>
       </c>
@@ -2527,13 +2661,16 @@
         <v>94</v>
       </c>
       <c r="I14" t="s">
+        <v>578</v>
+      </c>
+      <c r="J14" t="s">
         <v>95</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -2559,13 +2696,16 @@
         <v>102</v>
       </c>
       <c r="I15" t="s">
+        <v>577</v>
+      </c>
+      <c r="J15" t="s">
         <v>103</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -2591,13 +2731,16 @@
         <v>107</v>
       </c>
       <c r="I16" t="s">
+        <v>566</v>
+      </c>
+      <c r="J16" t="s">
         <v>108</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -2623,13 +2766,16 @@
         <v>112</v>
       </c>
       <c r="I17" t="s">
+        <v>581</v>
+      </c>
+      <c r="J17" t="s">
         <v>113</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -2655,13 +2801,16 @@
         <v>117</v>
       </c>
       <c r="I18" t="s">
+        <v>566</v>
+      </c>
+      <c r="J18" t="s">
         <v>118</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>120</v>
       </c>
@@ -2687,13 +2836,16 @@
         <v>123</v>
       </c>
       <c r="I19" t="s">
+        <v>573</v>
+      </c>
+      <c r="J19" t="s">
         <v>124</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -2719,13 +2871,16 @@
         <v>128</v>
       </c>
       <c r="I20" t="s">
+        <v>581</v>
+      </c>
+      <c r="J20" t="s">
         <v>129</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>131</v>
       </c>
@@ -2751,13 +2906,16 @@
         <v>133</v>
       </c>
       <c r="I21" t="s">
+        <v>577</v>
+      </c>
+      <c r="J21" t="s">
         <v>134</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -2783,13 +2941,16 @@
         <v>137</v>
       </c>
       <c r="I22" t="s">
+        <v>567</v>
+      </c>
+      <c r="J22" t="s">
         <v>138</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2815,13 +2976,16 @@
         <v>141</v>
       </c>
       <c r="I23" t="s">
+        <v>579</v>
+      </c>
+      <c r="J23" t="s">
         <v>142</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2847,13 +3011,16 @@
         <v>145</v>
       </c>
       <c r="I24" t="s">
+        <v>580</v>
+      </c>
+      <c r="J24" t="s">
         <v>146</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>148</v>
       </c>
@@ -2879,13 +3046,16 @@
         <v>152</v>
       </c>
       <c r="I25" t="s">
+        <v>573</v>
+      </c>
+      <c r="J25" t="s">
         <v>153</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>155</v>
       </c>
@@ -2911,13 +3081,16 @@
         <v>157</v>
       </c>
       <c r="I26" t="s">
+        <v>582</v>
+      </c>
+      <c r="J26" t="s">
         <v>158</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2943,13 +3116,16 @@
         <v>162</v>
       </c>
       <c r="I27" t="s">
+        <v>582</v>
+      </c>
+      <c r="J27" t="s">
         <v>163</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2975,13 +3151,16 @@
         <v>168</v>
       </c>
       <c r="I28" t="s">
+        <v>573</v>
+      </c>
+      <c r="J28" t="s">
         <v>169</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -3007,13 +3186,16 @@
         <v>174</v>
       </c>
       <c r="I29" t="s">
+        <v>577</v>
+      </c>
+      <c r="J29" t="s">
         <v>175</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -3039,13 +3221,16 @@
         <v>179</v>
       </c>
       <c r="I30" t="s">
+        <v>585</v>
+      </c>
+      <c r="J30" t="s">
         <v>180</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -3071,13 +3256,16 @@
         <v>183</v>
       </c>
       <c r="I31" t="s">
+        <v>566</v>
+      </c>
+      <c r="J31" t="s">
         <v>184</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>186</v>
       </c>
@@ -3103,13 +3291,16 @@
         <v>190</v>
       </c>
       <c r="I32" t="s">
+        <v>577</v>
+      </c>
+      <c r="J32" t="s">
         <v>191</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -3135,13 +3326,16 @@
         <v>194</v>
       </c>
       <c r="I33" t="s">
+        <v>586</v>
+      </c>
+      <c r="J33" t="s">
         <v>195</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -3167,13 +3361,16 @@
         <v>199</v>
       </c>
       <c r="I34" t="s">
+        <v>573</v>
+      </c>
+      <c r="J34" t="s">
         <v>200</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -3199,13 +3396,16 @@
         <v>205</v>
       </c>
       <c r="I35" t="s">
+        <v>568</v>
+      </c>
+      <c r="J35" t="s">
         <v>206</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -3231,13 +3431,16 @@
         <v>211</v>
       </c>
       <c r="I36" t="s">
+        <v>574</v>
+      </c>
+      <c r="J36" t="s">
         <v>212</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -3263,13 +3466,16 @@
         <v>217</v>
       </c>
       <c r="I37" t="s">
+        <v>579</v>
+      </c>
+      <c r="J37" t="s">
         <v>218</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -3295,13 +3501,16 @@
         <v>222</v>
       </c>
       <c r="I38" t="s">
+        <v>577</v>
+      </c>
+      <c r="J38" t="s">
         <v>223</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -3327,13 +3536,16 @@
         <v>226</v>
       </c>
       <c r="I39" t="s">
+        <v>574</v>
+      </c>
+      <c r="J39" t="s">
         <v>227</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -3359,13 +3571,16 @@
         <v>233</v>
       </c>
       <c r="I40" t="s">
+        <v>569</v>
+      </c>
+      <c r="J40" t="s">
         <v>234</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -3391,13 +3606,16 @@
         <v>239</v>
       </c>
       <c r="I41" t="s">
+        <v>576</v>
+      </c>
+      <c r="J41" t="s">
         <v>240</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -3423,13 +3641,16 @@
         <v>245</v>
       </c>
       <c r="I42" t="s">
+        <v>577</v>
+      </c>
+      <c r="J42" t="s">
         <v>246</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>248</v>
       </c>
@@ -3455,13 +3676,16 @@
         <v>250</v>
       </c>
       <c r="I43" t="s">
+        <v>577</v>
+      </c>
+      <c r="J43" t="s">
         <v>251</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -3487,13 +3711,16 @@
         <v>256</v>
       </c>
       <c r="I44" t="s">
+        <v>573</v>
+      </c>
+      <c r="J44" t="s">
         <v>257</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>259</v>
       </c>
@@ -3519,13 +3746,16 @@
         <v>262</v>
       </c>
       <c r="I45" t="s">
+        <v>576</v>
+      </c>
+      <c r="J45" t="s">
         <v>263</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -3551,13 +3781,16 @@
         <v>267</v>
       </c>
       <c r="I46" t="s">
+        <v>567</v>
+      </c>
+      <c r="J46" t="s">
         <v>268</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -3583,13 +3816,16 @@
         <v>273</v>
       </c>
       <c r="I47" t="s">
+        <v>579</v>
+      </c>
+      <c r="J47" t="s">
         <v>274</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -3615,13 +3851,16 @@
         <v>278</v>
       </c>
       <c r="I48" t="s">
+        <v>573</v>
+      </c>
+      <c r="J48" t="s">
         <v>279</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>281</v>
       </c>
@@ -3647,13 +3886,16 @@
         <v>283</v>
       </c>
       <c r="I49" t="s">
+        <v>582</v>
+      </c>
+      <c r="J49" t="s">
         <v>284</v>
       </c>
-      <c r="J49" t="s">
+      <c r="K49" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>286</v>
       </c>
@@ -3679,13 +3921,16 @@
         <v>288</v>
       </c>
       <c r="I50" t="s">
+        <v>581</v>
+      </c>
+      <c r="J50" t="s">
         <v>289</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -3711,13 +3956,16 @@
         <v>293</v>
       </c>
       <c r="I51" t="s">
+        <v>573</v>
+      </c>
+      <c r="J51" t="s">
         <v>294</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -3743,13 +3991,16 @@
         <v>297</v>
       </c>
       <c r="I52" t="s">
+        <v>574</v>
+      </c>
+      <c r="J52" t="s">
         <v>298</v>
       </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -3775,13 +4026,16 @@
         <v>301</v>
       </c>
       <c r="I53" t="s">
+        <v>574</v>
+      </c>
+      <c r="J53" t="s">
         <v>302</v>
       </c>
-      <c r="J53" t="s">
+      <c r="K53" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -3807,13 +4061,16 @@
         <v>305</v>
       </c>
       <c r="I54" t="s">
+        <v>570</v>
+      </c>
+      <c r="J54" t="s">
         <v>306</v>
       </c>
-      <c r="J54" t="s">
+      <c r="K54" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -3839,13 +4096,16 @@
         <v>311</v>
       </c>
       <c r="I55" t="s">
+        <v>573</v>
+      </c>
+      <c r="J55" t="s">
         <v>312</v>
       </c>
-      <c r="J55" t="s">
+      <c r="K55" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>314</v>
       </c>
@@ -3871,13 +4131,16 @@
         <v>316</v>
       </c>
       <c r="I56" t="s">
+        <v>576</v>
+      </c>
+      <c r="J56" t="s">
         <v>317</v>
       </c>
-      <c r="J56" t="s">
+      <c r="K56" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>319</v>
       </c>
@@ -3903,13 +4166,16 @@
         <v>321</v>
       </c>
       <c r="I57" t="s">
+        <v>577</v>
+      </c>
+      <c r="J57" t="s">
         <v>322</v>
       </c>
-      <c r="J57" t="s">
+      <c r="K57" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>324</v>
       </c>
@@ -3935,13 +4201,16 @@
         <v>326</v>
       </c>
       <c r="I58" t="s">
+        <v>573</v>
+      </c>
+      <c r="J58" t="s">
         <v>327</v>
       </c>
-      <c r="J58" t="s">
+      <c r="K58" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>329</v>
       </c>
@@ -3967,13 +4236,16 @@
         <v>331</v>
       </c>
       <c r="I59" t="s">
+        <v>581</v>
+      </c>
+      <c r="J59" t="s">
         <v>332</v>
       </c>
-      <c r="J59" t="s">
+      <c r="K59" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3999,13 +4271,16 @@
         <v>335</v>
       </c>
       <c r="I60" t="s">
+        <v>583</v>
+      </c>
+      <c r="J60" t="s">
         <v>336</v>
       </c>
-      <c r="J60" t="s">
+      <c r="K60" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>338</v>
       </c>
@@ -4031,13 +4306,16 @@
         <v>340</v>
       </c>
       <c r="I61" t="s">
+        <v>568</v>
+      </c>
+      <c r="J61" t="s">
         <v>341</v>
       </c>
-      <c r="J61" t="s">
+      <c r="K61" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -4063,13 +4341,16 @@
         <v>346</v>
       </c>
       <c r="I62" t="s">
+        <v>583</v>
+      </c>
+      <c r="J62" t="s">
         <v>347</v>
       </c>
-      <c r="J62" t="s">
+      <c r="K62" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -4095,13 +4376,16 @@
         <v>352</v>
       </c>
       <c r="I63" t="s">
+        <v>573</v>
+      </c>
+      <c r="J63" t="s">
         <v>353</v>
       </c>
-      <c r="J63" t="s">
+      <c r="K63" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>355</v>
       </c>
@@ -4127,13 +4411,16 @@
         <v>358</v>
       </c>
       <c r="I64" t="s">
+        <v>577</v>
+      </c>
+      <c r="J64" t="s">
         <v>359</v>
       </c>
-      <c r="J64" t="s">
+      <c r="K64" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -4159,13 +4446,16 @@
         <v>362</v>
       </c>
       <c r="I65" t="s">
+        <v>571</v>
+      </c>
+      <c r="J65" t="s">
         <v>363</v>
       </c>
-      <c r="J65" t="s">
+      <c r="K65" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>365</v>
       </c>
@@ -4191,13 +4481,16 @@
         <v>369</v>
       </c>
       <c r="I66" t="s">
+        <v>587</v>
+      </c>
+      <c r="J66" t="s">
         <v>370</v>
       </c>
-      <c r="J66" t="s">
+      <c r="K66" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>372</v>
       </c>
@@ -4223,13 +4516,16 @@
         <v>374</v>
       </c>
       <c r="I67" t="s">
+        <v>576</v>
+      </c>
+      <c r="J67" t="s">
         <v>375</v>
       </c>
-      <c r="J67" t="s">
+      <c r="K67" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -4255,13 +4551,16 @@
         <v>379</v>
       </c>
       <c r="I68" t="s">
+        <v>574</v>
+      </c>
+      <c r="J68" t="s">
         <v>380</v>
       </c>
-      <c r="J68" t="s">
+      <c r="K68" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -4287,13 +4586,16 @@
         <v>383</v>
       </c>
       <c r="I69" t="s">
+        <v>577</v>
+      </c>
+      <c r="J69" t="s">
         <v>384</v>
       </c>
-      <c r="J69" t="s">
+      <c r="K69" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>386</v>
       </c>
@@ -4319,13 +4621,16 @@
         <v>389</v>
       </c>
       <c r="I70" t="s">
+        <v>573</v>
+      </c>
+      <c r="J70" t="s">
         <v>390</v>
       </c>
-      <c r="J70" t="s">
+      <c r="K70" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -4351,13 +4656,16 @@
         <v>393</v>
       </c>
       <c r="I71" t="s">
+        <v>584</v>
+      </c>
+      <c r="J71" t="s">
         <v>394</v>
       </c>
-      <c r="J71" t="s">
+      <c r="K71" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -4383,13 +4691,16 @@
         <v>398</v>
       </c>
       <c r="I72" t="s">
+        <v>581</v>
+      </c>
+      <c r="J72" t="s">
         <v>399</v>
       </c>
-      <c r="J72" t="s">
+      <c r="K72" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>401</v>
       </c>
@@ -4415,13 +4726,16 @@
         <v>404</v>
       </c>
       <c r="I73" t="s">
+        <v>577</v>
+      </c>
+      <c r="J73" t="s">
         <v>405</v>
       </c>
-      <c r="J73" t="s">
+      <c r="K73" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -4447,13 +4761,16 @@
         <v>409</v>
       </c>
       <c r="I74" t="s">
+        <v>573</v>
+      </c>
+      <c r="J74" t="s">
         <v>410</v>
       </c>
-      <c r="J74" t="s">
+      <c r="K74" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>412</v>
       </c>
@@ -4479,13 +4796,16 @@
         <v>414</v>
       </c>
       <c r="I75" t="s">
+        <v>573</v>
+      </c>
+      <c r="J75" t="s">
         <v>415</v>
       </c>
-      <c r="J75" t="s">
+      <c r="K75" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>417</v>
       </c>
@@ -4511,13 +4831,16 @@
         <v>420</v>
       </c>
       <c r="I76" t="s">
+        <v>577</v>
+      </c>
+      <c r="J76" t="s">
         <v>421</v>
       </c>
-      <c r="J76" t="s">
+      <c r="K76" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -4543,13 +4866,16 @@
         <v>425</v>
       </c>
       <c r="I77" t="s">
+        <v>581</v>
+      </c>
+      <c r="J77" t="s">
         <v>426</v>
       </c>
-      <c r="J77" t="s">
+      <c r="K77" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -4575,13 +4901,16 @@
         <v>430</v>
       </c>
       <c r="I78" t="s">
+        <v>565</v>
+      </c>
+      <c r="J78" t="s">
         <v>431</v>
       </c>
-      <c r="J78" t="s">
+      <c r="K78" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>433</v>
       </c>
@@ -4607,13 +4936,16 @@
         <v>436</v>
       </c>
       <c r="I79" t="s">
+        <v>581</v>
+      </c>
+      <c r="J79" t="s">
         <v>437</v>
       </c>
-      <c r="J79" t="s">
+      <c r="K79" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -4639,13 +4971,16 @@
         <v>440</v>
       </c>
       <c r="I80" t="s">
+        <v>582</v>
+      </c>
+      <c r="J80" t="s">
         <v>441</v>
       </c>
-      <c r="J80" t="s">
+      <c r="K80" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>443</v>
       </c>
@@ -4671,13 +5006,16 @@
         <v>446</v>
       </c>
       <c r="I81" t="s">
+        <v>577</v>
+      </c>
+      <c r="J81" t="s">
         <v>447</v>
       </c>
-      <c r="J81" t="s">
+      <c r="K81" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -4703,13 +5041,16 @@
         <v>450</v>
       </c>
       <c r="I82" t="s">
+        <v>577</v>
+      </c>
+      <c r="J82" t="s">
         <v>451</v>
       </c>
-      <c r="J82" t="s">
+      <c r="K82" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -4735,13 +5076,16 @@
         <v>455</v>
       </c>
       <c r="I83" t="s">
+        <v>577</v>
+      </c>
+      <c r="J83" t="s">
         <v>456</v>
       </c>
-      <c r="J83" t="s">
+      <c r="K83" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -4767,13 +5111,16 @@
         <v>460</v>
       </c>
       <c r="I84" t="s">
+        <v>573</v>
+      </c>
+      <c r="J84" t="s">
         <v>461</v>
       </c>
-      <c r="J84" t="s">
+      <c r="K84" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -4799,13 +5146,16 @@
         <v>466</v>
       </c>
       <c r="I85" t="s">
+        <v>573</v>
+      </c>
+      <c r="J85" t="s">
         <v>467</v>
       </c>
-      <c r="J85" t="s">
+      <c r="K85" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>10</v>
       </c>
@@ -4831,13 +5181,16 @@
         <v>470</v>
       </c>
       <c r="I86" t="s">
+        <v>576</v>
+      </c>
+      <c r="J86" t="s">
         <v>471</v>
       </c>
-      <c r="J86" t="s">
+      <c r="K86" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>10</v>
       </c>
@@ -4863,13 +5216,16 @@
         <v>474</v>
       </c>
       <c r="I87" t="s">
+        <v>567</v>
+      </c>
+      <c r="J87" t="s">
         <v>475</v>
       </c>
-      <c r="J87" t="s">
+      <c r="K87" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -4895,13 +5251,16 @@
         <v>479</v>
       </c>
       <c r="I88" t="s">
+        <v>577</v>
+      </c>
+      <c r="J88" t="s">
         <v>480</v>
       </c>
-      <c r="J88" t="s">
+      <c r="K88" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>482</v>
       </c>
@@ -4927,13 +5286,16 @@
         <v>484</v>
       </c>
       <c r="I89" t="s">
+        <v>581</v>
+      </c>
+      <c r="J89" t="s">
         <v>485</v>
       </c>
-      <c r="J89" t="s">
+      <c r="K89" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>10</v>
       </c>
@@ -4959,13 +5321,16 @@
         <v>489</v>
       </c>
       <c r="I90" t="s">
+        <v>566</v>
+      </c>
+      <c r="J90" t="s">
         <v>490</v>
       </c>
-      <c r="J90" t="s">
+      <c r="K90" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>10</v>
       </c>
@@ -4991,13 +5356,16 @@
         <v>493</v>
       </c>
       <c r="I91" t="s">
+        <v>573</v>
+      </c>
+      <c r="J91" t="s">
         <v>494</v>
       </c>
-      <c r="J91" t="s">
+      <c r="K91" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>10</v>
       </c>
@@ -5023,13 +5391,16 @@
         <v>498</v>
       </c>
       <c r="I92" t="s">
+        <v>578</v>
+      </c>
+      <c r="J92" t="s">
         <v>499</v>
       </c>
-      <c r="J92" t="s">
+      <c r="K92" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>501</v>
       </c>
@@ -5055,13 +5426,16 @@
         <v>503</v>
       </c>
       <c r="I93" t="s">
+        <v>587</v>
+      </c>
+      <c r="J93" t="s">
         <v>504</v>
       </c>
-      <c r="J93" t="s">
+      <c r="K93" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>506</v>
       </c>
@@ -5087,13 +5461,16 @@
         <v>508</v>
       </c>
       <c r="I94" t="s">
+        <v>573</v>
+      </c>
+      <c r="J94" t="s">
         <v>509</v>
       </c>
-      <c r="J94" t="s">
+      <c r="K94" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -5119,13 +5496,16 @@
         <v>514</v>
       </c>
       <c r="I95" t="s">
+        <v>580</v>
+      </c>
+      <c r="J95" t="s">
         <v>515</v>
       </c>
-      <c r="J95" t="s">
+      <c r="K95" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>517</v>
       </c>
@@ -5151,13 +5531,16 @@
         <v>521</v>
       </c>
       <c r="I96" t="s">
+        <v>573</v>
+      </c>
+      <c r="J96" t="s">
         <v>522</v>
       </c>
-      <c r="J96" t="s">
+      <c r="K96" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>10</v>
       </c>
@@ -5183,13 +5566,16 @@
         <v>525</v>
       </c>
       <c r="I97" t="s">
+        <v>573</v>
+      </c>
+      <c r="J97" t="s">
         <v>526</v>
       </c>
-      <c r="J97" t="s">
+      <c r="K97" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>10</v>
       </c>
@@ -5215,13 +5601,16 @@
         <v>529</v>
       </c>
       <c r="I98" t="s">
+        <v>575</v>
+      </c>
+      <c r="J98" t="s">
         <v>530</v>
       </c>
-      <c r="J98" t="s">
+      <c r="K98" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>532</v>
       </c>
@@ -5247,13 +5636,16 @@
         <v>536</v>
       </c>
       <c r="I99" t="s">
+        <v>582</v>
+      </c>
+      <c r="J99" t="s">
         <v>537</v>
       </c>
-      <c r="J99" t="s">
+      <c r="K99" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>539</v>
       </c>
@@ -5279,13 +5671,16 @@
         <v>541</v>
       </c>
       <c r="I100" t="s">
+        <v>582</v>
+      </c>
+      <c r="J100" t="s">
         <v>542</v>
       </c>
-      <c r="J100" t="s">
+      <c r="K100" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>544</v>
       </c>
@@ -5311,13 +5706,16 @@
         <v>549</v>
       </c>
       <c r="I101" t="s">
+        <v>573</v>
+      </c>
+      <c r="J101" t="s">
         <v>550</v>
       </c>
-      <c r="J101" t="s">
+      <c r="K101" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>552</v>
       </c>
@@ -5343,13 +5741,16 @@
         <v>555</v>
       </c>
       <c r="I102" t="s">
+        <v>573</v>
+      </c>
+      <c r="J102" t="s">
         <v>556</v>
       </c>
-      <c r="J102" t="s">
+      <c r="K102" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>10</v>
       </c>
@@ -5375,13 +5776,33 @@
         <v>561</v>
       </c>
       <c r="I103" t="s">
+        <v>579</v>
+      </c>
+      <c r="J103" t="s">
         <v>562</v>
       </c>
-      <c r="J103" t="s">
+      <c r="K103" t="s">
         <v>563</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K103" xr:uid="{CEF96A98-240F-E541-BDB2-0551CB0EA07E}"/>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{504B95FC-C0B2-3142-939E-58B8B179258F}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{64106074-804E-B345-B82D-EBF4594F4E0D}"/>
+    <hyperlink ref="K4" r:id="rId3" xr:uid="{385C4F1F-BCB9-E048-9201-74C8E1850E2F}"/>
+    <hyperlink ref="K5" r:id="rId4" xr:uid="{14FE9F6B-553F-3F44-B29F-C313944CFE7F}"/>
+    <hyperlink ref="K6" r:id="rId5" xr:uid="{89806C48-4889-1C4F-9E1F-67CE30C12E32}"/>
+    <hyperlink ref="K9" r:id="rId6" xr:uid="{5F009573-EE43-5D49-9BAB-D2BED4B0C489}"/>
+    <hyperlink ref="K10" r:id="rId7" xr:uid="{ECCDD5E1-298E-C843-A53A-2F7221B75253}"/>
+    <hyperlink ref="K12" r:id="rId8" xr:uid="{9DB23B44-3A45-3642-BF5A-3BBF746F5F27}"/>
+    <hyperlink ref="K13" r:id="rId9" xr:uid="{47773718-91EA-4846-B2D3-CA17AB42CEFC}"/>
+    <hyperlink ref="K19" r:id="rId10" xr:uid="{C8E4B893-ECC0-044A-B00A-182D83019167}"/>
+    <hyperlink ref="K23" r:id="rId11" xr:uid="{E83776D6-FC83-584C-AB20-B528A6041C4E}"/>
+    <hyperlink ref="K24" r:id="rId12" xr:uid="{B26295B6-99B3-B843-98B3-120F9F469DB1}"/>
+    <hyperlink ref="K26" r:id="rId13" xr:uid="{BF6ACE49-331D-7941-A4C3-6B0C9FC8700F}"/>
+    <hyperlink ref="K30" r:id="rId14" xr:uid="{B93D6C5A-144A-0F47-ADF0-9153DBC0C672}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>